<commit_message>
Update rice production data (change most tables)
</commit_message>
<xml_diff>
--- a/Data/Rice_production_2014_GSO.xlsx
+++ b/Data/Rice_production_2014_GSO.xlsx
@@ -37,40 +37,40 @@
     <t xml:space="preserve">Rice yield (ton/ha)</t>
   </si>
   <si>
+    <t xml:space="preserve">Hanoi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vinh Phuc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bac Ninh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quang Ninh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hai Duong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hai Phong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hung Yen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thai Binh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ha Nam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nam Dinh</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ninh Binh</t>
   </si>
   <si>
-    <t xml:space="preserve">Nam Dinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ha Nam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vinh Phuc</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bac Giang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quang Ninh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hung Yen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hai Duong</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hanoi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thai Binh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hai Phong</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lang Son</t>
   </si>
 </sst>
 </file>
@@ -263,20 +263,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.2244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -296,109 +296,109 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="n">
-        <v>137800</v>
+        <v>332400</v>
       </c>
       <c r="C2" s="4" t="n">
-        <v>41900</v>
+        <v>101600</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>460900</v>
+        <v>1175500</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="n">
-        <v>165300</v>
+        <v>123800</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>76500</v>
+        <v>30800</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>914400</v>
+        <v>331200</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>5.88</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5.65</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="4" t="n">
-        <v>86100</v>
+        <v>82300</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>33800</v>
+        <v>36300</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>424500</v>
+        <v>439400</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>6.15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.04</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="4" t="n">
-        <v>123900</v>
+        <v>610200</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>30900</v>
+        <v>17200</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>308700</v>
+        <v>211300</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>5.23</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4.9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4" t="n">
-        <v>385000</v>
+        <v>165600</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>53200</v>
+        <v>63000</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>595300</v>
+        <v>742600</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>5.33</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5.94</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="4" t="n">
-        <v>610200</v>
+        <v>152700</v>
       </c>
       <c r="C7" s="4" t="n">
-        <v>17200</v>
+        <v>37500</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>211400</v>
+        <v>484700</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>4.92</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.29</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -406,100 +406,101 @@
         <v>92600</v>
       </c>
       <c r="C8" s="4" t="n">
-        <v>40400</v>
+        <v>39500</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>502700</v>
+        <v>489600</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>6.23</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.21</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="4" t="n">
-        <v>165600</v>
+        <v>157100</v>
       </c>
       <c r="C9" s="4" t="n">
-        <v>63400</v>
+        <v>80500</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>742800</v>
+        <v>1061900</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.56</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="4" t="n">
-        <v>332400</v>
+        <v>86200</v>
       </c>
       <c r="C10" s="4" t="n">
-        <v>102300</v>
+        <v>33400</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>1156300</v>
+        <v>401600</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>5.58</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5.96</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="4" t="n">
-        <v>157000</v>
+        <v>165300</v>
       </c>
       <c r="C11" s="4" t="n">
-        <v>80500</v>
+        <v>76300</v>
       </c>
       <c r="D11" s="4" t="n">
-        <v>1058400</v>
+        <v>937700</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>6.54</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.05</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="4" t="n">
-        <v>152700</v>
+        <v>137800</v>
       </c>
       <c r="C12" s="4" t="n">
-        <v>38400</v>
+        <v>41800</v>
       </c>
       <c r="D12" s="4" t="n">
-        <v>490100</v>
+        <v>484300</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>6.27</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.02</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="4" t="n">
-        <v>832100</v>
+        <v>385000</v>
       </c>
       <c r="C13" s="4" t="n">
-        <v>16100</v>
+        <v>53800</v>
       </c>
       <c r="D13" s="4" t="n">
-        <v>206600</v>
+        <v>626600</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>4.07</v>
-      </c>
-    </row>
+        <v>5.55</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>